<commit_message>
update congregations.py et iiif
</commit_message>
<xml_diff>
--- a/sources/iiif/collections.xlsx
+++ b/sources/iiif/collections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca\Documents\GitHub\SHERLOCK\sources\iiif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C522B98F-42C6-430C-93A2-D339073BFA53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16741E51-C5C7-4283-9B70-42D8784C4736}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DC105B8-4426-416F-89A5-0E95022221EB}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>collection</t>
   </si>
   <si>
-    <t>responsable</t>
-  </si>
-  <si>
     <t>type de collection</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Les 40 chanteurs montagnards</t>
   </si>
   <si>
-    <t>Nicolas Dufétel</t>
-  </si>
-  <si>
     <t>Publication numérisée.</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Gravures du Mercure Galant</t>
   </si>
   <si>
-    <t>Anne Piéjus</t>
-  </si>
-  <si>
     <t>Images</t>
   </si>
   <si>
@@ -118,13 +109,22 @@
   </si>
   <si>
     <t>Edition MEI</t>
+  </si>
+  <si>
+    <t>ea287800-4345-4649-af12-7253aa185f3f</t>
+  </si>
+  <si>
+    <t>7ebda3f2-cdfb-4f9c-9b86-0fb559bbfee5</t>
+  </si>
+  <si>
+    <t>responsable (uuid)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,12 +149,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -193,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -201,15 +202,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -219,10 +211,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -548,40 +550,43 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="38.109375" customWidth="1"/>
-    <col min="9" max="10" width="27" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="8"/>
+    <col min="5" max="5" width="19" style="8" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="38.109375" style="8" customWidth="1"/>
+    <col min="9" max="10" width="27" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="17.77734375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.45" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+    <row r="1" spans="1:12" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:12" ht="18" customHeight="1">
-      <c r="C2" s="9"/>
-      <c r="D2" s="8"/>
-      <c r="G2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="17.55" customHeight="1"/>
-    <row r="4" spans="1:12" ht="28.8">
+    <row r="3" spans="1:12" ht="17.55" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,103 +594,103 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.8">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="D7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="18" customHeight="1">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" customHeight="1">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -693,5 +698,6 @@
     <mergeCell ref="G2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rdfization des gravures du MG
</commit_message>
<xml_diff>
--- a/sources/iiif/collections.xlsx
+++ b/sources/iiif/collections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca\Documents\GitHub\SHERLOCK\sources\iiif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16741E51-C5C7-4283-9B70-42D8784C4736}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2B2F02-7C15-4E4A-86F9-03BD44CE8530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DC105B8-4426-416F-89A5-0E95022221EB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -63,9 +63,6 @@
     <t>lieu inconnu</t>
   </si>
   <si>
-    <t>GMG</t>
-  </si>
-  <si>
     <t>Gravures du Mercure Galant</t>
   </si>
   <si>
@@ -99,18 +96,6 @@
     <t>Edition</t>
   </si>
   <si>
-    <t>Partitions</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Partitions numérisées</t>
-  </si>
-  <si>
-    <t>Edition MEI</t>
-  </si>
-  <si>
     <t>ea287800-4345-4649-af12-7253aa185f3f</t>
   </si>
   <si>
@@ -118,6 +103,9 @@
   </si>
   <si>
     <t>responsable (uuid)</t>
+  </si>
+  <si>
+    <t>MGE</t>
   </si>
 </sst>
 </file>
@@ -214,9 +202,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -225,6 +210,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -547,24 +535,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3CE6F2-7211-4CDF-9292-163B353D125F}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="8"/>
-    <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="38.109375" style="8" customWidth="1"/>
-    <col min="9" max="10" width="27" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="17.77734375" style="8"/>
+    <col min="1" max="1" width="9.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="7"/>
+    <col min="5" max="5" width="19" style="7" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="38.109375" style="7" customWidth="1"/>
+    <col min="9" max="10" width="27" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="17.77734375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -576,14 +564,14 @@
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
-      <c r="G2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="G2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="17.55" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -594,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -606,91 +594,77 @@
         <v>4</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>